<commit_message>
Added all 5 Haar like features. Added Excel sheet to keep track of calculations used.:
</commit_message>
<xml_diff>
--- a/docs/New Microsoft Excel Worksheet.xlsx
+++ b/docs/New Microsoft Excel Worksheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="81">
   <si>
     <t>a</t>
   </si>
@@ -42,18 +42,242 @@
     <t>number of variations in 24x24</t>
   </si>
   <si>
-    <t>total possible sizes on 1 axis</t>
-  </si>
-  <si>
-    <t>24 - feature_total_size + 1</t>
+    <t>Type A/1</t>
+  </si>
+  <si>
+    <t>white tleft</t>
+  </si>
+  <si>
+    <t>corners of rectangle</t>
+  </si>
+  <si>
+    <t>coordinate</t>
+  </si>
+  <si>
+    <t>white tright</t>
+  </si>
+  <si>
+    <t>white bleft</t>
+  </si>
+  <si>
+    <t>black tleft</t>
+  </si>
+  <si>
+    <t>black tright</t>
+  </si>
+  <si>
+    <t>black bleft</t>
+  </si>
+  <si>
+    <t>white bright</t>
+  </si>
+  <si>
+    <t>black  bright</t>
+  </si>
+  <si>
+    <t>(I, j)</t>
+  </si>
+  <si>
+    <t>given i, j, h, w</t>
+  </si>
+  <si>
+    <t>(I, j+w/2-1)</t>
+  </si>
+  <si>
+    <t>(i+h-1, j)</t>
+  </si>
+  <si>
+    <t>(i+h-1, j+w/2-1)</t>
+  </si>
+  <si>
+    <t>(I, j+w/2)</t>
+  </si>
+  <si>
+    <t>(I, j+w-1)</t>
+  </si>
+  <si>
+    <t>(i+h-1, j+w/2)</t>
+  </si>
+  <si>
+    <t>Type B/2</t>
+  </si>
+  <si>
+    <t>left white tleft</t>
+  </si>
+  <si>
+    <t>left white tright</t>
+  </si>
+  <si>
+    <t>left white bleft</t>
+  </si>
+  <si>
+    <t>left white bright</t>
+  </si>
+  <si>
+    <t>right white tleft</t>
+  </si>
+  <si>
+    <t>right white tright</t>
+  </si>
+  <si>
+    <t>right white bleft</t>
+  </si>
+  <si>
+    <t>right white bright</t>
+  </si>
+  <si>
+    <t>(I, j+w/3-1)</t>
+  </si>
+  <si>
+    <t>(I, j+w/3)</t>
+  </si>
+  <si>
+    <t>(I, j+2w/3-1)</t>
+  </si>
+  <si>
+    <t>(I, j+2w/3)</t>
+  </si>
+  <si>
+    <t>(i+h-1,  j+w/3-1)</t>
+  </si>
+  <si>
+    <t>(i+h-1, j+w/3)</t>
+  </si>
+  <si>
+    <t>(i+h-1, 2w/3-1)</t>
+  </si>
+  <si>
+    <t>(i+h-1, j+2w/3)</t>
+  </si>
+  <si>
+    <t>(i+h-1, j+w-1)</t>
+  </si>
+  <si>
+    <t>Type C/3</t>
+  </si>
+  <si>
+    <t>(i+h/2-1, j)</t>
+  </si>
+  <si>
+    <t>(i+h/2-1, j+w-1)</t>
+  </si>
+  <si>
+    <t>(I+h/2, j)</t>
+  </si>
+  <si>
+    <t>(I+h/2, j+w-1)</t>
+  </si>
+  <si>
+    <t>Type D/4</t>
+  </si>
+  <si>
+    <t>top white tleft</t>
+  </si>
+  <si>
+    <t>top white tright</t>
+  </si>
+  <si>
+    <t>top white bleft</t>
+  </si>
+  <si>
+    <t>top white bright</t>
+  </si>
+  <si>
+    <t>bottom white tleft</t>
+  </si>
+  <si>
+    <t>bottom white tright</t>
+  </si>
+  <si>
+    <t>bottom white bleft</t>
+  </si>
+  <si>
+    <t>bottom white bright</t>
+  </si>
+  <si>
+    <t>(i+h/3-1, j)</t>
+  </si>
+  <si>
+    <t>(I+h/3, j)</t>
+  </si>
+  <si>
+    <t>(I+2h/3, j)</t>
+  </si>
+  <si>
+    <t>(i+2h/3-1, j)</t>
+  </si>
+  <si>
+    <t>(i+h/3-1,  j+w-1)</t>
+  </si>
+  <si>
+    <t>(I+h/3, j+w-1)</t>
+  </si>
+  <si>
+    <t>(i+2h/3-1, j+w-1)</t>
+  </si>
+  <si>
+    <t>(I+2h/3, j+w-1)</t>
+  </si>
+  <si>
+    <t>Type E/5</t>
+  </si>
+  <si>
+    <t>top black tleft</t>
+  </si>
+  <si>
+    <t>top black tright</t>
+  </si>
+  <si>
+    <t>top black bleft</t>
+  </si>
+  <si>
+    <t>top black  bright</t>
+  </si>
+  <si>
+    <t>bottom black tleft</t>
+  </si>
+  <si>
+    <t>bottom black tright</t>
+  </si>
+  <si>
+    <t>bottom black bleft</t>
+  </si>
+  <si>
+    <t>bottom black  bright</t>
+  </si>
+  <si>
+    <t>(i+h/2-1, j+w/2-1)</t>
+  </si>
+  <si>
+    <t>(i+h/2-1, j+w/2)</t>
+  </si>
+  <si>
+    <t>(i+h/2, j)</t>
+  </si>
+  <si>
+    <t>(i+h/2, j+w/2-1)</t>
+  </si>
+  <si>
+    <t>(i+h/2, j+w/2)</t>
+  </si>
+  <si>
+    <t>(i+h/2, j+w-1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,7 +293,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -77,12 +301,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -110,8 +351,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1733550</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>19617</xdr:rowOff>
     </xdr:to>
@@ -412,79 +653,601 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A10:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F1" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>27600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>27600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>20736</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>43200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <v>27600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>43200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14">
-        <v>27600</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15">
-        <v>20736</v>
+      <c r="B19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>